<commit_message>
Tests prix mementis + debut test div
</commit_message>
<xml_diff>
--- a/Excel/casMedian2.xlsx
+++ b/Excel/casMedian2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\PEPSI\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C392C22-6820-4BA4-B029-9D1A048C7497}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8314456E-BAF9-4D4F-8179-178C4FCD8E14}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7440" xr2:uid="{5172E695-FFD0-4A81-8853-8CB156196831}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="302">
   <si>
     <t>1215.38</t>
   </si>
@@ -1420,15 +1420,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8926E1A2-95A1-4361-8542-D3980DDE6A70}">
   <dimension ref="A1:AK96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W12" workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25"/>
+    <sheetView tabSelected="1" topLeftCell="T16" workbookViewId="0">
+      <selection activeCell="AC30" sqref="AC20:AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.6328125" customWidth="1"/>
     <col min="27" max="27" width="13.453125" customWidth="1"/>
-    <col min="29" max="29" width="14.08984375" customWidth="1"/>
+    <col min="29" max="29" width="19" customWidth="1"/>
     <col min="30" max="30" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3907,6 +3907,13 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
+      <c r="AC31" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD31">
+        <f>AVERAGE(AB19:AB30)</f>
+        <v>1.0087000002743947</v>
+      </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
@@ -6755,12 +6762,12 @@
     </row>
     <row r="65" spans="28:35" x14ac:dyDescent="0.35">
       <c r="AB65" s="11">
-        <f>(AVERAGE(AC34:AC45)-SUM(AE49:AE60))</f>
-        <v>0.18073200100538256</v>
+        <f>(AD31-AF61)</f>
+        <v>9.1932001663930007E-2</v>
       </c>
       <c r="AD65">
         <f>$AD$3 * (1+MAX(0,AB65))</f>
-        <v>118.07320010053826</v>
+        <v>109.193200166393</v>
       </c>
       <c r="AI65" s="9"/>
     </row>

</xml_diff>